<commit_message>
Diagrammi ER delle tabelle da creare dai sorgenti
</commit_message>
<xml_diff>
--- a/Documentazione/INFO SITI/siti e commenti.xlsx
+++ b/Documentazione/INFO SITI/siti e commenti.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wissel\OneDrive\Desktop\università\MAGISTRALE\Ing.Dati\Homeworks\Homework5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wissel\OneDrive\Desktop\università\MAGISTRALE\Ing.Dati\Homework 5- repo\Web-Scraping-homework5\Documentazione\INFO SITI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372676EF-5350-4F66-8DA6-15A39F4180DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE4212B-4774-43F1-95F1-9F8CF9111346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58C6E6E7-DA5C-4E52-99B3-A440589593F4}"/>
+    <workbookView minimized="1" xWindow="-28020" yWindow="3570" windowWidth="17280" windowHeight="8880" xr2:uid="{58C6E6E7-DA5C-4E52-99B3-A440589593F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -332,25 +332,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -372,6 +357,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -690,7 +691,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,109 +702,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="15" customFormat="1" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="15" customFormat="1" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="15" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="15" customFormat="1" ht="49.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="49.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" s="15" customFormat="1" ht="29.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:3" s="10" customFormat="1" ht="29.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="14"/>
-    </row>
-    <row r="7" spans="1:3" s="12" customFormat="1" ht="29.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:3" s="7" customFormat="1" ht="29.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" s="12" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="22" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" s="7" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <v>-1465</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="1" t="s">
         <v>24</v>
       </c>
@@ -812,60 +813,60 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="11"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="1" t="s">
         <v>35</v>
       </c>
@@ -874,7 +875,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
@@ -889,8 +890,9 @@
     <hyperlink ref="A4" r:id="rId1" display="https://www.gov.uk/" xr:uid="{F5FC69BD-379E-4CF0-AF9B-EE264E5D5545}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{31783097-A0FD-4B8B-B968-66AA93C804FD}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{B4126270-1F4D-4701-B535-AA4F9407478E}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{18A9D812-F0B8-42F3-A2B0-7335D615C08C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>